<commit_message>
corrige errores en requirements.txt
</commit_message>
<xml_diff>
--- a/static/reporte_diario.xlsx
+++ b/static/reporte_diario.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45753</v>
+        <v>45776</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -475,19 +475,19 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dieta Hiperproteica</t>
+          <t>3.5 ONZAS</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>60000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45753</v>
+        <v>45776</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -496,82 +496,82 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dieta Normal</t>
+          <t>Alta en Fibra</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3" t="n">
-        <v>60000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45753</v>
+        <v>45776</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dieta Hipoglucida</t>
+          <t>Astringente</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E4" t="n">
-        <v>36000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45753</v>
+        <v>45776</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Dieta Renal</t>
+          <t>Blanda</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>181</v>
       </c>
       <c r="E5" t="n">
-        <v>36000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45753</v>
+        <v>45776</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Dieta Normal</t>
+          <t>Coronaria</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="E6" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45754</v>
+        <v>45776</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -580,95 +580,95 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Dieta Hiperproteica</t>
+          <t>Hepatica</t>
         </is>
       </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45759</v>
+        <v>45776</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Refrigerio</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Dieta Hiperproteica</t>
+          <t>Hipercalorica</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>10500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45759</v>
+        <v>45776</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Refrigerio</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Dieta Hipograsa</t>
+          <t>Hiperproteica</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E9" t="n">
-        <v>10500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45759</v>
+        <v>45776</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Refrigerio</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dieta Liquida Clara</t>
+          <t>Hipo Grasa</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E10" t="n">
-        <v>10500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45760</v>
+        <v>45776</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Otra: deliciosa</t>
+          <t>Hipoglucida</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>12</v>
+        <v>347</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -676,170 +676,1976 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45760</v>
+        <v>45776</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Dieta Hiperproteica</t>
+          <t>Hipograsa</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="E12" t="n">
-        <v>15000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45760</v>
+        <v>45776</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Dieta Liquida Clara</t>
+          <t>Hiposodica</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>338</v>
       </c>
       <c r="E13" t="n">
-        <v>15000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45760</v>
+        <v>45776</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Dieta Normal</t>
+          <t>Liquida Clara</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="E14" t="n">
-        <v>15000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45760</v>
+        <v>45776</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Refrigerio</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Dieta Hiperproteica</t>
+          <t>Liquida Total</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="E15" t="n">
-        <v>31500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45760</v>
+        <v>45776</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Refrigerio</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Dieta Liquida Clara</t>
+          <t>Liquida Total Nectar</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
+        <v>114</v>
       </c>
       <c r="E16" t="n">
-        <v>31500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45760</v>
+        <v>45776</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Refrigerio</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Dieta Normal</t>
+          <t>Liquida total Miel</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E17" t="n">
-        <v>31500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45761</v>
+        <v>45776</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Dieta Hiposódica</t>
+          <t>LÍQUIDA TOTAL 140 CC</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E18" t="n">
-        <v>27000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45761</v>
+        <v>45776</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Otra: Con sal</t>
+          <t>LÍQUIDA TOTAL MIEL 140 CC</t>
         </is>
       </c>
       <c r="D19" t="n">
+        <v>22</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>LÍQUIDA TOTAL NÉCTAR 140 CC</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>18</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Líquida Total 140 Cc</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Líquida Total Miel 140 CC</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Líquida Total Néctar 140 CC</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>NADA VÍA ORAL</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>543</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Nada Vía Oral</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>14</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>614</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Pequena Semiblanda</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>57</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Renal Dialisis</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>106</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Renal PRE Dialisis</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>7</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Renal SIN Dialisis</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>52</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Semiblanda</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>290</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Semiblanda Pequena</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>5</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Todo Pure</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>27</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Almuerzo</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>5</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>3.0 ONZAS</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>3.0 ONZAS LQ</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>3.5 ONZAS</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>7</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>5 Onzas</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Alta en Fibra</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Astringente</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>31</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Blanda</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>174</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Coronaria</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>183</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Dieta Renal</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Hepatica</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>2</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Hipercalorica</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>10</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Hiperproteica</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>20</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Hipo Grasa</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>24</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Hipoglucida</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>360</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Hipograsa</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>99</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Hiposodica</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>350</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Liquida Clara</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>66</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Liquida Total</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>61</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Liquida Total Nectar</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>119</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Liquida total Miel</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>26</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>LÍQUIDA TOTAL 140 CC</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>4</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>LÍQUIDA TOTAL MIEL 140 CC</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>30</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>LÍQUIDA TOTAL NÉCTAR 140 CC</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>13</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Líquida Total 140 Cc</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Líquida Total Miel 3</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Líquida Total Néctar 140 CC</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
         <v>3</v>
       </c>
-      <c r="E19" t="n">
-        <v>27000</v>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>NADA VÍA ORAL</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>304</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>614</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Pequena Semiblanda</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>57</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Renal Dialisis</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>107</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Renal PRE Dialisis</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>10</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Renal SIN Dialisis</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>48</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Semiblanda</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>288</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Semiblanda Pequena</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>6</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Todo Pure</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>28</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>2</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>3.0 ONZAS</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>2</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>3.5 ONZAS</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>3</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Alta en Fibra</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>3</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Astringente</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>29</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Blanda</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>205</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Coronaria</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>207</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Hepatica</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>3</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Hipercalorica</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>10</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Hiperproteica</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>22</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Hipo Grasa</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>29</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Hipoglucida</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>381</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Hipograsa</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>88</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Hiposodica</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>382</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Liquida Clara</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>61</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Liquida Total</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>70</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Liquida Total Nectar</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>112</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Liquida total Miel</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>29</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>LÍQUIDA TOTAL 140 CC</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>3</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>LÍQUIDA TOTAL MIEL 140 CC</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>27</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>LÍQUIDA TOTAL NÉCTAR 140 CC</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>18</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Líquida Total 140 Cc</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>1</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Líquida Total Miel 140 CC</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>1</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Líquida Total Néctar 140 CC</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>3</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>NADA VÍA ORAL</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>413</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>646</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Pequena Semiblanda</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>52</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Renal Dialisis</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>106</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Renal PRE Dialisis</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>14</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Renal SIN Dialisis</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>47</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Semiblanda</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>299</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Semiblanda Pequena</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>11</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Todo Pure</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>28</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>100</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="n">
+        <v>45777</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>1</v>
+      </c>
+      <c r="E104" t="n">
+        <v>15808</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>45777</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Semiblanda</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>1</v>
+      </c>
+      <c r="E105" t="n">
+        <v>15808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primera versión funcional de Ordéna con login, menú y vistas activas
</commit_message>
<xml_diff>
--- a/static/reporte_diario.xlsx
+++ b/static/reporte_diario.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,16 +470,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Almuerzo</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Astringente</t>
+          <t>Hiposodica</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -491,16 +491,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Blanda</t>
+          <t>3.0 ONZAS LQ</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -512,16 +512,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Coronaria</t>
+          <t>3.0 Onzas</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -533,16 +533,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Hepatica</t>
+          <t>3.5 Onzas</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -554,12 +554,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Hipercalorica</t>
+          <t>5 Onzas</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -575,16 +575,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hiperproteica</t>
+          <t>Alta en Fibra</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -596,16 +596,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Hipo Grasa</t>
+          <t>Astringente</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -617,16 +617,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hipoglucida</t>
+          <t>Blanda</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>12</v>
+        <v>174</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -638,16 +638,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Hiposodica</t>
+          <t>Coronaria</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>28</v>
+        <v>183</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -659,16 +659,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Liquida Clara</t>
+          <t>Hepatica</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -680,16 +680,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Liquida Total</t>
+          <t>Hipercalorica</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -701,16 +701,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Liquida Total 140 Cc</t>
+          <t>Hiperproteica</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -722,16 +722,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Liquida Total Miel 140 Cc</t>
+          <t>Hipo Grasa</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -743,16 +743,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Liquida Total Nectar</t>
+          <t>Hipoglucida</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>9</v>
+        <v>359</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -764,16 +764,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Liquida Total Nectar 140 Cc</t>
+          <t>Hipograsa</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -785,16 +785,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Liquida total Miel</t>
+          <t>Hiposodica</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>350</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -806,16 +806,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Liquida Clara</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -827,16 +827,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Renal Dialisis</t>
+          <t>Liquida Total</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -848,12 +848,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Renal PRE Dialisis</t>
+          <t>Liquida Total 140 Cc</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -869,16 +869,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Semiblanda</t>
+          <t>Liquida Total Miel 140 Cc</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -890,16 +890,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Semiblanda Pequena</t>
+          <t>Liquida Total Miel 3</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -911,18 +911,732 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Desayuno</t>
+          <t>Cena</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>Liquida Total Nectar</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>119</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Liquida Total Nectar 140 Cc</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>16</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Liquida total Miel</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>26</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Nada Via Oral</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>304</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>613</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Pequena Semiblanda</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>57</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Renal Dialisis</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>107</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Renal PRE Dialisis</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>10</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Renal SIN Dialisis</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>48</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Semiblanda</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>287</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Semiblanda Pequena</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>6</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
           <t>Todo Pure</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D34" t="n">
+        <v>28</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Cena</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
         <v>2</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Astringente</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>3</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Blanda</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>19</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Coronaria</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>15</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Hepatica</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Hipercalorica</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Hiperproteica</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Hipo Grasa</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>6</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Hipoglucida</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>12</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Hiposodica</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>28</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Liquida Clara</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>4</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Liquida Total</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>7</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Liquida Total 140 Cc</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Liquida Total Miel 140 Cc</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>2</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Liquida Total Nectar</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>9</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Liquida Total Nectar 140 Cc</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>2</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Liquida total Miel</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>3</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>57</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Renal Dialisis</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>4</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Renal PRE Dialisis</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>5</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Semiblanda</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>28</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Semiblanda Pequena</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>4</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Desayuno</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Todo Pure</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>2</v>
+      </c>
+      <c r="E57" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización final para presentación: filtrado por CDS, carga manual, mejoras visuales
</commit_message>
<xml_diff>
--- a/static/reporte_diario.xlsx
+++ b/static/reporte_diario.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,20 +466,20 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Almuerzo</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hiposodica</t>
+          <t>3.0 Onzas</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -487,20 +487,20 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3.0 ONZAS LQ</t>
+          <t>3.5 Onzas</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -508,20 +508,20 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3.0 Onzas</t>
+          <t>Alta en Fibra</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -529,20 +529,20 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3.5 Onzas</t>
+          <t>Astringente</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -550,20 +550,20 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5 Onzas</t>
+          <t>Blanda</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>205</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -571,20 +571,20 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Alta en Fibra</t>
+          <t>Coronaria</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>207</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -592,20 +592,20 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Astringente</t>
+          <t>Hepatica</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -613,20 +613,20 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Blanda</t>
+          <t>Hipercalorica</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>174</v>
+        <v>10</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -634,20 +634,20 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Coronaria</t>
+          <t>Hiperproteica</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>183</v>
+        <v>22</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -655,20 +655,20 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Hepatica</t>
+          <t>Hipo Grasa</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -676,20 +676,20 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Hipercalorica</t>
+          <t>Hipoglucida</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>10</v>
+        <v>381</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -697,20 +697,20 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Hiperproteica</t>
+          <t>Hipograsa</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -718,20 +718,20 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Hipo Grasa</t>
+          <t>Hiposodica</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>24</v>
+        <v>382</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -739,20 +739,20 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Hipoglucida</t>
+          <t>Liquida Clara</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>359</v>
+        <v>61</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -760,20 +760,20 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Hipograsa</t>
+          <t>Liquida Total</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -781,20 +781,20 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Hiposodica</t>
+          <t>Liquida Total 140 Cc</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>350</v>
+        <v>4</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -802,20 +802,20 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Liquida Clara</t>
+          <t>Liquida Total Miel 140 Cc</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -823,20 +823,20 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Liquida Total</t>
+          <t>Liquida Total Nectar</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -844,20 +844,20 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Liquida Total 140 Cc</t>
+          <t>Liquida Total Nectar 140 Cc</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -865,20 +865,20 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Liquida Total Miel 140 Cc</t>
+          <t>Liquida total Miel</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -886,20 +886,20 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Liquida Total Miel 3</t>
+          <t>Nada Via Oral</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>413</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -907,20 +907,20 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Liquida Total Nectar</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>119</v>
+        <v>646</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -928,20 +928,20 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Liquida Total Nectar 140 Cc</t>
+          <t>Pequena Semiblanda</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -949,20 +949,20 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Liquida total Miel</t>
+          <t>Renal Dialisis</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -970,20 +970,20 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Nada Via Oral</t>
+          <t>Renal PRE Dialisis</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>304</v>
+        <v>14</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -991,20 +991,20 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Renal SIN Dialisis</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>613</v>
+        <v>47</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -1012,20 +1012,20 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Pequena Semiblanda</t>
+          <t>Semiblanda</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>57</v>
+        <v>299</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -1033,20 +1033,20 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Renal Dialisis</t>
+          <t>Semiblanda Pequena</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>107</v>
+        <v>11</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -1054,20 +1054,20 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Renal PRE Dialisis</t>
+          <t>Todo Pure</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -1075,568 +1075,22 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45792</v>
+        <v>45822</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Cena</t>
+          <t>Desayuno</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Renal SIN Dialisis</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Cena</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Semiblanda</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>287</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Cena</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Semiblanda Pequena</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>6</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Cena</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Todo Pure</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>28</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Cena</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>2</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Astringente</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>3</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Blanda</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>19</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Coronaria</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>15</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Hepatica</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Hipercalorica</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>1</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Hiperproteica</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>2</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Hipo Grasa</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
-        <v>6</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Hipoglucida</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>12</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Hiposodica</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>28</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Liquida Clara</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>4</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Liquida Total</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>7</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Liquida Total 140 Cc</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>1</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Liquida Total Miel 140 Cc</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>2</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Liquida Total Nectar</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>9</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Liquida Total Nectar 140 Cc</t>
-        </is>
-      </c>
-      <c r="D50" t="n">
-        <v>2</v>
-      </c>
-      <c r="E50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Liquida total Miel</t>
-        </is>
-      </c>
-      <c r="D51" t="n">
-        <v>3</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>57</v>
-      </c>
-      <c r="E52" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Renal Dialisis</t>
-        </is>
-      </c>
-      <c r="D53" t="n">
-        <v>4</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Renal PRE Dialisis</t>
-        </is>
-      </c>
-      <c r="D54" t="n">
-        <v>5</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Semiblanda</t>
-        </is>
-      </c>
-      <c r="D55" t="n">
-        <v>28</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Semiblanda Pequena</t>
-        </is>
-      </c>
-      <c r="D56" t="n">
-        <v>4</v>
-      </c>
-      <c r="E56" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="2" t="n">
-        <v>45792</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Desayuno</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Todo Pure</t>
-        </is>
-      </c>
-      <c r="D57" t="n">
-        <v>2</v>
-      </c>
-      <c r="E57" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>